<commit_message>
Updated excel table with results
</commit_message>
<xml_diff>
--- a/results/Models_results_table.xlsx
+++ b/results/Models_results_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\source\repos\RO2_TSP\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\source\repos\RO2_TSP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF2740C-CAAF-4E19-88E4-1A12EAA58178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021851DB-A309-4B17-98D2-DFC06C65EF4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9432" yWindow="2496" windowWidth="17280" windowHeight="8964" xr2:uid="{F6A87395-A6BC-4D82-82B7-09765E513F51}"/>
+    <workbookView xWindow="-12975" yWindow="4050" windowWidth="21600" windowHeight="11385" xr2:uid="{F6A87395-A6BC-4D82-82B7-09765E513F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Nome istanza</t>
   </si>
@@ -126,10 +126,43 @@
     <t>N.B. time_limit parameter has been set to 3600s (1h) and verbosity to minimum level (LOW = 0).</t>
   </si>
   <si>
-    <t>3607,007 (time_limit)</t>
-  </si>
-  <si>
-    <t>3638,713 (time_limit)</t>
+    <t>Seed number</t>
+  </si>
+  <si>
+    <t>berlin52 (4)</t>
+  </si>
+  <si>
+    <t>berlin52 (5)</t>
+  </si>
+  <si>
+    <t>eil51 (4)</t>
+  </si>
+  <si>
+    <t>eil51 (5)</t>
+  </si>
+  <si>
+    <t>eil76 (4)</t>
+  </si>
+  <si>
+    <t>eil76 (5)</t>
+  </si>
+  <si>
+    <t>pr76 (4)</t>
+  </si>
+  <si>
+    <t>pr76 (5)</t>
+  </si>
+  <si>
+    <t>st70 (4)</t>
+  </si>
+  <si>
+    <t>st70 (5)</t>
+  </si>
+  <si>
+    <t>att48 (4)</t>
+  </si>
+  <si>
+    <t>att48 (5)</t>
   </si>
 </sst>
 </file>
@@ -212,10 +245,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01EAF5BE-C14D-42C0-AF8C-8E445F1C107E}" name="Tabella1" displayName="Tabella1" ref="A1:E30" totalsRowShown="0">
-  <autoFilter ref="A1:E30" xr:uid="{6DC7176A-D0EB-4952-A8E7-C62E3F317DCA}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01EAF5BE-C14D-42C0-AF8C-8E445F1C107E}" name="Tabella1" displayName="Tabella1" ref="A1:F42" totalsRowShown="0">
+  <autoFilter ref="A1:F42" xr:uid="{6DC7176A-D0EB-4952-A8E7-C62E3F317DCA}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CFB15A07-94F2-4C55-8B6C-1D25C6DD7C29}" name="Nome istanza"/>
+    <tableColumn id="6" xr3:uid="{E7506ACA-5B80-4873-8B46-70089239FC13}" name="Seed number"/>
     <tableColumn id="2" xr3:uid="{9AEF4C77-0263-4D78-98F2-EECB17E74CAB}" name="MTZ_STATIC (1)" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{3A2E36D7-70E3-4729-830D-E1729716A6DD}" name="MTZ_LAZY (2)" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{3E978640-250A-40E9-BCF1-9DD9BF65CA13}" name="MTZ_SUBTOUR_SIZE_2 (3)" dataDxfId="1"/>
@@ -522,487 +556,723 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C745AED4-C5FF-4D99-9225-3EAA71D62680}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>224.66900000000001</v>
+      <c r="B2">
+        <v>123456</v>
       </c>
       <c r="C2" s="1">
-        <v>1806.2449999999999</v>
+        <v>343.68599999999998</v>
       </c>
       <c r="D2" s="1">
-        <v>633.44000000000005</v>
+        <v>1574.8440000000001</v>
       </c>
       <c r="E2" s="1">
-        <v>12.348000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>188.52699999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>223.99100000000001</v>
+      <c r="B3">
+        <v>234567</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <v>12.503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>222.03299999999999</v>
+      <c r="B4">
+        <v>345678</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>12.548999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <f>AVERAGE(B2:B4)</f>
-        <v>223.56433333333334</v>
-      </c>
-      <c r="C5" s="1">
-        <f>AVERAGE(C2:C4)</f>
-        <v>1806.2449999999999</v>
-      </c>
-      <c r="D5" s="1">
-        <f>AVERAGE(D2:D4)</f>
-        <v>633.44000000000005</v>
-      </c>
-      <c r="E5" s="1">
-        <f>AVERAGE(E2:E4)</f>
-        <v>12.466666666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>456789</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>567890</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <f>AVERAGE(C2:C4)</f>
+        <v>343.68599999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <f>AVERAGE(D2:D4)</f>
+        <v>1574.8440000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <f>AVERAGE(E2:E4)</f>
+        <v>188.52699999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <f>AVERAGE(F2:F4)</f>
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>3.1709999999999998</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.302</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.629</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4.08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>123456</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.9319999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.2270000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.026</v>
+      </c>
+      <c r="F9" s="1">
+        <v>14.930999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>2.8820000000000001</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.345</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4.3259999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B10">
+        <v>234567</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.6120000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>2.8809999999999998</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.2969999999999999</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="E9" s="1">
-        <v>4.165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11">
+        <v>345678</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.7470000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.135</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6.2779999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>456789</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.032</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.093</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.228</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10.893000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>567890</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.903</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.169</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5.2690000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
-        <f>AVERAGE(B7:B9)</f>
-        <v>2.9779999999999998</v>
-      </c>
-      <c r="C10" s="1">
-        <f>AVERAGE(C7:C9)</f>
-        <v>1.3146666666666667</v>
-      </c>
-      <c r="D10" s="1">
-        <f>AVERAGE(D7:D9)</f>
-        <v>0.6333333333333333</v>
-      </c>
-      <c r="E10" s="1">
-        <f>AVERAGE(E7:E9)</f>
-        <v>4.1903333333333324</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C14" s="1">
+        <f>AVERAGE(C9:C13)</f>
+        <v>2.2452000000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <f>AVERAGE(D9:D13)</f>
+        <v>1.5512000000000001</v>
+      </c>
+      <c r="E14" s="1">
+        <f>AVERAGE(E9:E13)</f>
+        <v>0.85940000000000016</v>
+      </c>
+      <c r="F14" s="1">
+        <f>AVERAGE(F9:F13)</f>
+        <v>8.6001999999999992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1">
-        <v>2.5670000000000002</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.528</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="E12" s="1">
-        <v>11.27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B16">
+        <v>123456</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.234</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1.258</v>
+      </c>
+      <c r="F16" s="1">
+        <v>12.707000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1">
-        <v>2.4809999999999999</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.45</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="E13" s="1">
-        <v>10.662000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B17">
+        <v>234567</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6.6479999999999997</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.2669999999999999</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="F17" s="1">
+        <v>13.901999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1">
-        <v>2.4969999999999999</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1.494</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.51100000000000001</v>
-      </c>
-      <c r="E14" s="1">
-        <v>10.657</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B18">
+        <v>345678</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7.1840000000000002</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.8010000000000002</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F18" s="1">
+        <v>15.926</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>456789</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.0730000000000004</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.8089999999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>13.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>567890</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5.681</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.3740000000000001</v>
+      </c>
+      <c r="F20" s="1">
+        <v>10.712999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1">
-        <f>AVERAGE(B12:B14)</f>
-        <v>2.5150000000000001</v>
-      </c>
-      <c r="C15" s="1">
-        <f>AVERAGE(C12:C14)</f>
-        <v>1.4906666666666666</v>
-      </c>
-      <c r="D15" s="1">
-        <f>AVERAGE(D12:D14)</f>
-        <v>0.51166666666666671</v>
-      </c>
-      <c r="E15" s="1">
-        <f>AVERAGE(E12:E14)</f>
-        <v>10.863</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C21" s="1">
+        <f>AVERAGE(C16:C20)</f>
+        <v>5.1581999999999999</v>
+      </c>
+      <c r="D21" s="1">
+        <f>AVERAGE(D16:D20)</f>
+        <v>2.3752</v>
+      </c>
+      <c r="E21" s="1">
+        <f>AVERAGE(E16:E20)</f>
+        <v>1.0422</v>
+      </c>
+      <c r="F21" s="1">
+        <f>AVERAGE(F16:F20)</f>
+        <v>13.259600000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1">
-        <v>8.9079999999999995</v>
-      </c>
-      <c r="C17" s="1">
-        <v>13.125999999999999</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1.3160000000000001</v>
-      </c>
-      <c r="E17" s="1">
-        <v>86.206999999999994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B23">
+        <v>123456</v>
+      </c>
+      <c r="C23" s="1">
+        <v>15.988</v>
+      </c>
+      <c r="D23" s="1">
+        <v>16.571999999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.5470000000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <v>67.094999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
-        <v>8.3390000000000004</v>
-      </c>
-      <c r="C18" s="1">
-        <v>12.154</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1.2729999999999999</v>
-      </c>
-      <c r="E18" s="1">
-        <v>85.453000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B24">
+        <v>234567</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9.0739999999999998</v>
+      </c>
+      <c r="D24" s="1">
+        <v>49.904000000000003</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F24" s="1">
+        <v>42.875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1">
-        <v>8.0690000000000008</v>
-      </c>
-      <c r="C19" s="1">
-        <v>12.08</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1.262</v>
-      </c>
-      <c r="E19" s="1">
-        <v>83.903999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B25">
+        <v>345678</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8.3740000000000006</v>
+      </c>
+      <c r="D25" s="1">
+        <v>12.467000000000001</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.0749999999999993</v>
+      </c>
+      <c r="F25" s="1">
+        <v>61.814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>456789</v>
+      </c>
+      <c r="C26" s="1">
+        <v>30.766999999999999</v>
+      </c>
+      <c r="D26" s="1">
+        <v>26.428000000000001</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2.1120000000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>64.004000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>567890</v>
+      </c>
+      <c r="C27" s="1">
+        <v>26.114000000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>25.07</v>
+      </c>
+      <c r="E27" s="1">
+        <v>4.7469999999999999</v>
+      </c>
+      <c r="F27" s="1">
+        <v>68.021000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="1">
-        <f>AVERAGE(B17:B19)</f>
-        <v>8.4386666666666681</v>
-      </c>
-      <c r="C20" s="1">
-        <f>AVERAGE(C17:C19)</f>
-        <v>12.453333333333333</v>
-      </c>
-      <c r="D20" s="1">
-        <f>AVERAGE(D17:D19)</f>
-        <v>1.2836666666666667</v>
-      </c>
-      <c r="E20" s="1">
-        <f>AVERAGE(E17:E19)</f>
-        <v>85.188000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="C28" s="1">
+        <f>AVERAGE(C23:C27)</f>
+        <v>18.063400000000001</v>
+      </c>
+      <c r="D28" s="1">
+        <f>AVERAGE(D23:D27)</f>
+        <v>26.088200000000001</v>
+      </c>
+      <c r="E28" s="1">
+        <f>AVERAGE(E23:E27)</f>
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="F28" s="1">
+        <f>AVERAGE(F23:F27)</f>
+        <v>60.761800000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1">
-        <v>1038.991</v>
-      </c>
-      <c r="C22" s="1">
-        <v>308.91699999999997</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="1">
-        <v>211.946</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B30">
+        <v>123456</v>
+      </c>
+      <c r="C30" s="1">
+        <v>968.476</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1108.567</v>
+      </c>
+      <c r="E30" s="1">
+        <v>519.27200000000005</v>
+      </c>
+      <c r="F30" s="1">
+        <v>389.358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1">
-        <v>303.88600000000002</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1">
-        <v>213.29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B31">
+        <v>234567</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1">
-        <v>313.54300000000001</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1">
-        <v>210.048</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B32">
+        <v>345678</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>456789</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>567890</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="1">
-        <f>AVERAGE(B22:B24)</f>
-        <v>1038.991</v>
-      </c>
-      <c r="C25" s="1">
-        <f>AVERAGE(C22:C24)</f>
-        <v>308.78199999999998</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1">
-        <f>AVERAGE(E22:E24)</f>
-        <v>211.76133333333334</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="C35" s="1">
+        <f>AVERAGE(C30:C34)</f>
+        <v>968.476</v>
+      </c>
+      <c r="D35" s="1">
+        <f>AVERAGE(D30:D34)</f>
+        <v>1108.567</v>
+      </c>
+      <c r="E35" s="1">
+        <f>AVERAGE(E30:E34)</f>
+        <v>519.27200000000005</v>
+      </c>
+      <c r="F35" s="1">
+        <f>AVERAGE(F30:F34)</f>
+        <v>389.358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="1">
-        <v>1119.7149999999999</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="1">
-        <v>44.182000000000002</v>
-      </c>
-      <c r="E27" s="1">
-        <v>41.319000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B37">
+        <v>123456</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3601.47</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4480.5540000000001</v>
+      </c>
+      <c r="E37" s="1">
+        <v>99.613</v>
+      </c>
+      <c r="F37" s="1">
+        <v>34.718000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1">
-        <v>40.965000000000003</v>
-      </c>
-      <c r="E28" s="1">
-        <v>41.521999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B38">
+        <v>234567</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1">
-        <v>42.069000000000003</v>
-      </c>
-      <c r="E29" s="1">
-        <v>39.838000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B39">
+        <v>345678</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>456789</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>567890</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="1">
-        <f>AVERAGE(B27:B29)</f>
-        <v>1119.7149999999999</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1">
-        <f>AVERAGE(D27:D29)</f>
-        <v>42.405333333333338</v>
-      </c>
-      <c r="E30" s="1">
-        <f>AVERAGE(E27:E29)</f>
-        <v>40.893000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1">
+        <f>AVERAGE(E37:E39)</f>
+        <v>99.613</v>
+      </c>
+      <c r="F42" s="1">
+        <f>AVERAGE(F37:F39)</f>
+        <v>34.718000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B10:E10">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="C14:F14">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFF6161"/>
+        <color rgb="FF00D661"/>
+        <color rgb="FFFF4F4F"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF4F4F"/>
         <color rgb="FF00D661"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1012,14 +1282,16 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFF4F4F"/>
+        <color rgb="FFFF6161"/>
         <color rgb="FF00D661"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:F21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1029,7 +1301,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:E15">
+  <conditionalFormatting sqref="C28:F28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1039,7 +1311,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:E20">
+  <conditionalFormatting sqref="E42:F42 C42">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1049,7 +1321,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:E30 B30">
+  <conditionalFormatting sqref="C7:F7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1059,7 +1331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:E5">
+  <conditionalFormatting sqref="C35:D35 F35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1069,7 +1341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:C25 E25">
+  <conditionalFormatting sqref="C35:F35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Implemented Benders method, updated results table.
</commit_message>
<xml_diff>
--- a/results/Models_results_table.xlsx
+++ b/results/Models_results_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\source\repos\RO2_TSP\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\source\repos\RO2_TSP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021851DB-A309-4B17-98D2-DFC06C65EF4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C552F2D0-2CAE-446A-BA6D-CC031B21E975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12975" yWindow="4050" windowWidth="21600" windowHeight="11385" xr2:uid="{F6A87395-A6BC-4D82-82B7-09765E513F51}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6A87395-A6BC-4D82-82B7-09765E513F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Nome istanza</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>att48 (5)</t>
+  </si>
+  <si>
+    <t>Test setup specs: Intel Core i5 4570 @ 3.2 Ghz (3.39 Ghz average), 16 GB @ 1333 Mhz, "Max performance" profile set in Windows 10 power management.</t>
   </si>
 </sst>
 </file>
@@ -556,23 +559,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C745AED4-C5FF-4D99-9225-3EAA71D62680}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -612,7 +615,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -624,7 +627,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -636,7 +639,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -648,7 +651,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -660,7 +663,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -681,13 +684,13 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -707,7 +710,7 @@
         <v>14.930999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -727,7 +730,7 @@
         <v>5.63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -747,7 +750,7 @@
         <v>6.2779999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -767,7 +770,7 @@
         <v>10.893000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -787,7 +790,7 @@
         <v>5.2690000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -808,13 +811,13 @@
         <v>8.6001999999999992</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -834,7 +837,7 @@
         <v>12.707000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -854,7 +857,7 @@
         <v>13.901999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -874,7 +877,7 @@
         <v>15.926</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -894,7 +897,7 @@
         <v>13.05</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -914,7 +917,7 @@
         <v>10.712999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -935,13 +938,13 @@
         <v>13.259600000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -961,7 +964,7 @@
         <v>67.094999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -981,7 +984,7 @@
         <v>42.875</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>61.814</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>64.004000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>68.021000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1062,13 +1065,13 @@
         <v>60.761800000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>389.358</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +1103,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1113,7 +1116,7 @@
       <c r="F32" s="1"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1126,7 +1129,7 @@
       <c r="F33" s="1"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1139,7 +1142,7 @@
       <c r="F34" s="1"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1160,13 +1163,13 @@
         <v>389.358</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>34.718000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1198,7 +1201,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1210,7 +1213,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1222,7 +1225,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1234,7 +1237,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -1249,9 +1252,14 @@
         <v>34.718000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>